<commit_message>
inclui las librerias seaborn y las plotly
</commit_message>
<xml_diff>
--- a/BASE_DE_DATOS - TAREAS/REGRESION_ML_EN/Plantilla_Prediccion_Consumo.xlsx
+++ b/BASE_DE_DATOS - TAREAS/REGRESION_ML_EN/Plantilla_Prediccion_Consumo.xlsx
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -53,8 +53,13 @@
       <b val="1"/>
       <sz val="11"/>
     </font>
+    <font>
+      <i val="1"/>
+      <color rgb="00006400"/>
+      <sz val="9"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -79,6 +84,12 @@
         <bgColor rgb="00FFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C6EFCE"/>
+        <bgColor rgb="00C6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -98,7 +109,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -119,6 +130,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -516,9 +531,9 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="inlineStr">
-        <is>
-          <t>Creado: 2025-11-20 01:23:07</t>
+      <c r="A3" s="10" t="inlineStr">
+        <is>
+          <t>Última predicción: 2025-11-25 10:49:00</t>
         </is>
       </c>
     </row>
@@ -584,7 +599,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G6" s="8" t="inlineStr"/>
+      <c r="G6" s="11" t="n">
+        <v>824.6900000000001</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="7" t="n">
@@ -611,7 +628,9 @@
           <t>Sí</t>
         </is>
       </c>
-      <c r="G7" s="8" t="inlineStr"/>
+      <c r="G7" s="11" t="n">
+        <v>1008.26</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="7" t="n">
@@ -638,7 +657,9 @@
           <t>No</t>
         </is>
       </c>
-      <c r="G8" s="8" t="inlineStr"/>
+      <c r="G8" s="11" t="n">
+        <v>824.6900000000001</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="7" t="n">
@@ -808,9 +829,7 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-    </row>
+    <row r="6"/>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
@@ -839,9 +858,7 @@
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-    </row>
+    <row r="11"/>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
@@ -863,9 +880,7 @@
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-    </row>
+    <row r="15"/>
     <row r="16">
       <c r="A16" s="9" t="inlineStr">
         <is>
@@ -904,13 +919,11 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t xml:space="preserve">  - Entrenado: 2025-11-20 01:08:53</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr"/>
-    </row>
+          <t xml:space="preserve">  - Entrenado: 2025-11-25 09:18:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="22"/>
     <row r="23">
       <c r="A23" s="9" t="inlineStr">
         <is>

</xml_diff>